<commit_message>
renaming + trained parameters for OCR speedometer
</commit_message>
<xml_diff>
--- a/DataDigitResults.xlsx
+++ b/DataDigitResults.xlsx
@@ -25,13 +25,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -54,8 +60,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -336,90 +343,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A897"/>
+  <dimension ref="A1:G897"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A860" workbookViewId="0">
-      <selection activeCell="A898" sqref="A898"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="M129" sqref="M129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1021,7 +1029,7 @@
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
@@ -1036,7 +1044,7 @@
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
@@ -1051,7 +1059,7 @@
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
@@ -1066,7 +1074,7 @@
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
@@ -2386,7 +2394,7 @@
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A409">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.25">
@@ -2401,7 +2409,7 @@
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A412">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.25">
@@ -2416,7 +2424,7 @@
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A415">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="416" spans="1:1" x14ac:dyDescent="0.25">
@@ -2431,7 +2439,7 @@
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A418">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.25">
@@ -3751,7 +3759,7 @@
     </row>
     <row r="682" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A682">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="683" spans="1:1" x14ac:dyDescent="0.25">
@@ -3766,7 +3774,7 @@
     </row>
     <row r="685" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A685">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="686" spans="1:1" x14ac:dyDescent="0.25">
@@ -3781,7 +3789,7 @@
     </row>
     <row r="688" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A688">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="689" spans="1:1" x14ac:dyDescent="0.25">
@@ -3796,7 +3804,7 @@
     </row>
     <row r="691" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A691">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="692" spans="1:1" x14ac:dyDescent="0.25">
@@ -4831,5 +4839,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>